<commit_message>
Completed DSPortalTest, HomeTest, LoginTest and the corresponding setups in Util files.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DSAlgoTestData.xlsx
+++ b/src/test/resources/testdata/DSAlgoTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18012" windowHeight="3372" tabRatio="933" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18012" windowHeight="3372" tabRatio="933" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HomeDD" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="177">
   <si>
     <t>username</t>
   </si>
@@ -586,6 +586,33 @@
   </si>
   <si>
     <t>array</t>
+  </si>
+  <si>
+    <t>linked-list</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>Linked List</t>
+  </si>
+  <si>
+    <t>Tree</t>
+  </si>
+  <si>
+    <t>Data Structures-Introduction</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,39 +1035,60 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1799,7 +1847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>69</v>
       </c>
@@ -3087,52 +3135,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+        <v>168</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3145,7 +3217,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3397,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -3470,7 +3542,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>